<commit_message>
Adds manufacturer and model to the XNAT session for each batch of files
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_scanned.xlsx
+++ b/tests/fixtures/basic_scanned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44322CCD-8213-B943-8B80-18D393C1FA98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF81DC89-FA7D-B846-957D-DE60D2E8A9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5540" yWindow="1760" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5120" yWindow="5660" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
   <si>
     <t>File</t>
   </si>
@@ -227,6 +227,15 @@
   </si>
   <si>
     <t>tests/fixtures/basic/DOE^JOHN-002304/20200312HeadCT/Head CT/image-00001.dcm</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>ManufacturerModelName</t>
+  </si>
+  <si>
+    <t>StationName</t>
   </si>
 </sst>
 </file>
@@ -566,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCC7506-3A8B-3C43-9E0E-9F3B5EB91639}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -577,7 +586,7 @@
     <col min="2" max="2" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -606,28 +615,37 @@
         <v>5</v>
       </c>
       <c r="J1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" t="s">
+        <v>70</v>
+      </c>
+      <c r="L1" t="s">
         <v>23</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" t="s">
         <v>25</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>24</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>41</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>63</v>
       </c>
@@ -641,7 +659,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -663,29 +681,29 @@
       <c r="I3" t="s">
         <v>38</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>26</v>
       </c>
-      <c r="K3" t="s">
+      <c r="N3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="O3" t="s">
         <v>27</v>
       </c>
-      <c r="M3" t="s">
+      <c r="P3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" t="s">
+      <c r="Q3" t="s">
         <v>11</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>39</v>
       </c>
-      <c r="P3" t="s">
+      <c r="S3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -707,29 +725,29 @@
       <c r="I4" t="s">
         <v>38</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>26</v>
       </c>
-      <c r="K4" t="s">
+      <c r="N4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" t="s">
+      <c r="O4" t="s">
         <v>27</v>
       </c>
-      <c r="M4" t="s">
+      <c r="P4" t="s">
         <v>13</v>
       </c>
-      <c r="N4" t="s">
+      <c r="Q4" t="s">
         <v>11</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>39</v>
       </c>
-      <c r="P4" t="s">
+      <c r="S4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -751,29 +769,29 @@
       <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>26</v>
       </c>
-      <c r="K5" t="s">
+      <c r="N5" t="s">
         <v>12</v>
       </c>
-      <c r="L5" t="s">
+      <c r="O5" t="s">
         <v>27</v>
       </c>
-      <c r="M5" t="s">
+      <c r="P5" t="s">
         <v>13</v>
       </c>
-      <c r="N5" t="s">
+      <c r="Q5" t="s">
         <v>11</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>47</v>
       </c>
-      <c r="P5" t="s">
+      <c r="S5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -795,29 +813,29 @@
       <c r="I6" t="s">
         <v>46</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>26</v>
       </c>
-      <c r="K6" t="s">
+      <c r="N6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="O6" t="s">
         <v>27</v>
       </c>
-      <c r="M6" t="s">
+      <c r="P6" t="s">
         <v>13</v>
       </c>
-      <c r="N6" t="s">
+      <c r="Q6" t="s">
         <v>11</v>
       </c>
-      <c r="O6" t="s">
+      <c r="R6" t="s">
         <v>47</v>
       </c>
-      <c r="P6" t="s">
+      <c r="S6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -839,29 +857,29 @@
       <c r="I7" t="s">
         <v>46</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>26</v>
       </c>
-      <c r="K7" t="s">
+      <c r="N7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="O7" t="s">
         <v>27</v>
       </c>
-      <c r="M7" t="s">
+      <c r="P7" t="s">
         <v>13</v>
       </c>
-      <c r="N7" t="s">
+      <c r="Q7" t="s">
         <v>11</v>
       </c>
-      <c r="O7" t="s">
+      <c r="R7" t="s">
         <v>47</v>
       </c>
-      <c r="P7" t="s">
+      <c r="S7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>53</v>
       </c>
@@ -875,7 +893,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -889,7 +907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -911,29 +929,29 @@
       <c r="I10" t="s">
         <v>51</v>
       </c>
-      <c r="J10" t="s">
+      <c r="L10" t="s">
         <v>26</v>
       </c>
-      <c r="K10" t="s">
+      <c r="N10" t="s">
         <v>18</v>
       </c>
-      <c r="L10" t="s">
+      <c r="O10" t="s">
         <v>27</v>
       </c>
-      <c r="M10" t="s">
+      <c r="P10" t="s">
         <v>19</v>
       </c>
-      <c r="N10" t="s">
+      <c r="Q10" t="s">
         <v>17</v>
       </c>
-      <c r="O10" t="s">
+      <c r="R10" t="s">
         <v>51</v>
       </c>
-      <c r="P10" t="s">
+      <c r="S10" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>56</v>
       </c>
@@ -947,7 +965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -969,29 +987,29 @@
       <c r="I12" t="s">
         <v>51</v>
       </c>
-      <c r="J12" t="s">
+      <c r="L12" t="s">
         <v>26</v>
       </c>
-      <c r="K12" t="s">
+      <c r="N12" t="s">
         <v>20</v>
       </c>
-      <c r="L12" t="s">
+      <c r="O12" t="s">
         <v>27</v>
       </c>
-      <c r="M12" t="s">
+      <c r="P12" t="s">
         <v>19</v>
       </c>
-      <c r="N12" t="s">
+      <c r="Q12" t="s">
         <v>17</v>
       </c>
-      <c r="O12" t="s">
+      <c r="R12" t="s">
         <v>51</v>
       </c>
-      <c r="P12" t="s">
+      <c r="S12" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>58</v>
       </c>
@@ -1005,7 +1023,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1027,29 +1045,29 @@
       <c r="I14" t="s">
         <v>51</v>
       </c>
-      <c r="J14" t="s">
+      <c r="L14" t="s">
         <v>26</v>
       </c>
-      <c r="K14" t="s">
+      <c r="N14" t="s">
         <v>21</v>
       </c>
-      <c r="L14" t="s">
+      <c r="O14" t="s">
         <v>27</v>
       </c>
-      <c r="M14" t="s">
+      <c r="P14" t="s">
         <v>19</v>
       </c>
-      <c r="N14" t="s">
+      <c r="Q14" t="s">
         <v>17</v>
       </c>
-      <c r="O14" t="s">
+      <c r="R14" t="s">
         <v>51</v>
       </c>
-      <c r="P14" t="s">
+      <c r="S14" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>60</v>
       </c>
@@ -1063,7 +1081,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1085,25 +1103,25 @@
       <c r="I16" t="s">
         <v>40</v>
       </c>
-      <c r="J16" t="s">
+      <c r="L16" t="s">
         <v>26</v>
       </c>
-      <c r="K16" t="s">
+      <c r="N16" t="s">
         <v>15</v>
       </c>
-      <c r="L16" t="s">
+      <c r="O16" t="s">
         <v>27</v>
       </c>
-      <c r="M16" t="s">
+      <c r="P16" t="s">
         <v>16</v>
       </c>
-      <c r="N16" t="s">
+      <c r="Q16" t="s">
         <v>14</v>
       </c>
-      <c r="O16" t="s">
+      <c r="R16" t="s">
         <v>40</v>
       </c>
-      <c r="P16" t="s">
+      <c r="S16" t="s">
         <v>52</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Sorted out a lot of inconsistency with how spreadsheet <-> FileMatch marshalling works. Still not passing scan tests
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_scanned.xlsx
+++ b/tests/fixtures/basic_scanned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF81DC89-FA7D-B846-957D-DE60D2E8A9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AAC367-8515-4447-A07B-B49B792FFBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="5660" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5120" yWindow="3300" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="2" r:id="rId1"/>
@@ -91,15 +91,6 @@
     <t>Pattern</t>
   </si>
   <si>
-    <t>Modality</t>
-  </si>
-  <si>
-    <t>StudyDescription</t>
-  </si>
-  <si>
-    <t>StudyDate</t>
-  </si>
-  <si>
     <t>CT</t>
   </si>
   <si>
@@ -229,13 +220,22 @@
     <t>tests/fixtures/basic/DOE^JOHN-002304/20200312HeadCT/Head CT/image-00001.dcm</t>
   </si>
   <si>
-    <t>Manufacturer</t>
-  </si>
-  <si>
-    <t>ManufacturerModelName</t>
-  </si>
-  <si>
-    <t>StationName</t>
+    <t>DICOM:Manufacturer</t>
+  </si>
+  <si>
+    <t>DICOM:ManufacturerModelName</t>
+  </si>
+  <si>
+    <t>DICOM:Modality</t>
+  </si>
+  <si>
+    <t>DICOM:StationName</t>
+  </si>
+  <si>
+    <t>DICOM:StudyDate</t>
+  </si>
+  <si>
+    <t>DICOM:StudyDescription</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -594,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -603,54 +603,54 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="J1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" t="s">
         <v>69</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>70</v>
       </c>
-      <c r="L1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>71</v>
-      </c>
-      <c r="N1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O1" t="s">
-        <v>24</v>
       </c>
       <c r="P1" t="s">
         <v>6</v>
       </c>
       <c r="Q1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="R1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="S1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -664,31 +664,31 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N3" t="s">
         <v>12</v>
       </c>
       <c r="O3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s">
         <v>13</v>
@@ -697,10 +697,10 @@
         <v>11</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="S3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -708,31 +708,31 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
       </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N4" t="s">
         <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P4" t="s">
         <v>13</v>
@@ -741,10 +741,10 @@
         <v>11</v>
       </c>
       <c r="R4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="S4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
@@ -752,31 +752,31 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
       </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N5" t="s">
         <v>12</v>
       </c>
       <c r="O5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
         <v>13</v>
@@ -785,10 +785,10 @@
         <v>11</v>
       </c>
       <c r="R5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
@@ -796,31 +796,31 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
       </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N6" t="s">
         <v>12</v>
       </c>
       <c r="O6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
         <v>13</v>
@@ -829,10 +829,10 @@
         <v>11</v>
       </c>
       <c r="R6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.2">
@@ -840,31 +840,31 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="L7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N7" t="s">
         <v>12</v>
       </c>
       <c r="O7" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
         <v>13</v>
@@ -873,18 +873,18 @@
         <v>11</v>
       </c>
       <c r="R7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="S7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -895,10 +895,10 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -912,31 +912,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N10" t="s">
         <v>18</v>
       </c>
       <c r="O10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s">
         <v>19</v>
@@ -945,18 +945,18 @@
         <v>17</v>
       </c>
       <c r="R10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -970,31 +970,31 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
       </c>
+      <c r="F12" t="s">
+        <v>17</v>
+      </c>
       <c r="G12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>20</v>
-      </c>
-      <c r="I12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N12" t="s">
         <v>20</v>
       </c>
       <c r="O12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P12" t="s">
         <v>19</v>
@@ -1003,18 +1003,18 @@
         <v>17</v>
       </c>
       <c r="R12" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1028,31 +1028,31 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>10</v>
       </c>
+      <c r="F14" t="s">
+        <v>17</v>
+      </c>
       <c r="G14" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="H14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="L14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N14" t="s">
         <v>21</v>
       </c>
       <c r="O14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P14" t="s">
         <v>19</v>
@@ -1061,18 +1061,18 @@
         <v>17</v>
       </c>
       <c r="R14" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="S14" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1086,31 +1086,31 @@
         <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D16" t="s">
         <v>10</v>
       </c>
+      <c r="F16" t="s">
+        <v>14</v>
+      </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="L16" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="N16" t="s">
         <v>15</v>
       </c>
       <c r="O16" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="P16" t="s">
         <v>16</v>
@@ -1119,18 +1119,18 @@
         <v>14</v>
       </c>
       <c r="R16" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="S16" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added SeriesNumber to the default DICOM metadata and spreadsheets
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_scanned.xlsx
+++ b/tests/fixtures/basic_scanned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AAC367-8515-4447-A07B-B49B792FFBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A02E9E3-24C7-774F-855A-DBF03EEDDB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="3300" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="1520" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
   <si>
     <t>File</t>
   </si>
@@ -236,6 +236,9 @@
   </si>
   <si>
     <t>DICOM:StudyDescription</t>
+  </si>
+  <si>
+    <t>DICOM:SeriesNumber</t>
   </si>
 </sst>
 </file>
@@ -575,10 +578,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCC7506-3A8B-3C43-9E0E-9F3B5EB91639}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -586,7 +589,7 @@
     <col min="2" max="2" width="69" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -624,28 +627,31 @@
         <v>68</v>
       </c>
       <c r="M1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N1" t="s">
         <v>69</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>70</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>71</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>33</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>38</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>60</v>
       </c>
@@ -659,7 +665,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -684,26 +690,29 @@
       <c r="L3" t="s">
         <v>23</v>
       </c>
-      <c r="N3" t="s">
+      <c r="M3">
+        <v>6168</v>
+      </c>
+      <c r="O3" t="s">
         <v>12</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>24</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>11</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>36</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -728,26 +737,29 @@
       <c r="L4" t="s">
         <v>23</v>
       </c>
-      <c r="N4" t="s">
+      <c r="M4">
+        <v>6168</v>
+      </c>
+      <c r="O4" t="s">
         <v>12</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>24</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>11</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>36</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -772,26 +784,29 @@
       <c r="L5" t="s">
         <v>23</v>
       </c>
-      <c r="N5" t="s">
+      <c r="M5">
+        <v>6168</v>
+      </c>
+      <c r="O5" t="s">
         <v>12</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>24</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>13</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>11</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>44</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -816,26 +831,29 @@
       <c r="L6" t="s">
         <v>23</v>
       </c>
-      <c r="N6" t="s">
+      <c r="M6">
+        <v>6168</v>
+      </c>
+      <c r="O6" t="s">
         <v>12</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>24</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>13</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>11</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>44</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -860,26 +878,29 @@
       <c r="L7" t="s">
         <v>23</v>
       </c>
-      <c r="N7" t="s">
+      <c r="M7">
+        <v>6168</v>
+      </c>
+      <c r="O7" t="s">
         <v>12</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>24</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>13</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>11</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>44</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>50</v>
       </c>
@@ -893,7 +914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>51</v>
       </c>
@@ -907,7 +928,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -932,26 +953,29 @@
       <c r="L10" t="s">
         <v>23</v>
       </c>
-      <c r="N10" t="s">
+      <c r="M10">
+        <v>6168</v>
+      </c>
+      <c r="O10" t="s">
         <v>18</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>24</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>19</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>17</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>48</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -965,7 +989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -990,26 +1014,29 @@
       <c r="L12" t="s">
         <v>23</v>
       </c>
-      <c r="N12" t="s">
+      <c r="M12">
+        <v>6168</v>
+      </c>
+      <c r="O12" t="s">
         <v>20</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>24</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" t="s">
         <v>19</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>17</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>48</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>55</v>
       </c>
@@ -1023,7 +1050,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1048,26 +1075,29 @@
       <c r="L14" t="s">
         <v>23</v>
       </c>
-      <c r="N14" t="s">
+      <c r="M14">
+        <v>6168</v>
+      </c>
+      <c r="O14" t="s">
         <v>21</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>24</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>17</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>48</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>57</v>
       </c>
@@ -1081,7 +1111,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>9</v>
       </c>
@@ -1106,22 +1136,25 @@
       <c r="L16" t="s">
         <v>23</v>
       </c>
-      <c r="N16" t="s">
+      <c r="M16">
+        <v>6168</v>
+      </c>
+      <c r="O16" t="s">
         <v>15</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>24</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" t="s">
         <v>16</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>14</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" t="s">
         <v>37</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored the scan function so that it calls collate_uploads so that we can check whether all the files in a scan have the same series number to use as the scan id. (It appears that in real world datasets, they don't.)
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_scanned.xlsx
+++ b/tests/fixtures/basic_scanned.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A02E9E3-24C7-774F-855A-DBF03EEDDB65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040A1F9-69D2-4241-9826-59686092553B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6280" yWindow="1520" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
   <si>
     <t>File</t>
   </si>
@@ -239,6 +239,21 @@
   </si>
   <si>
     <t>DICOM:SeriesNumber</t>
+  </si>
+  <si>
+    <t>002304_CT1</t>
+  </si>
+  <si>
+    <t>397829_CT1</t>
+  </si>
+  <si>
+    <t>397829_CT2</t>
+  </si>
+  <si>
+    <t>397829_CT3</t>
+  </si>
+  <si>
+    <t>038945_CT1</t>
   </si>
 </sst>
 </file>
@@ -581,7 +596,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:M1048576"/>
+      <selection activeCell="I2" sqref="I2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -652,17 +667,53 @@
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <v>6168</v>
+      </c>
+      <c r="O2" t="s">
+        <v>12</v>
+      </c>
+      <c r="P2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
@@ -670,10 +721,10 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -687,6 +738,9 @@
       <c r="H3" t="s">
         <v>35</v>
       </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
       <c r="L3" t="s">
         <v>23</v>
       </c>
@@ -709,7 +763,7 @@
         <v>36</v>
       </c>
       <c r="T3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
@@ -717,10 +771,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -732,7 +786,10 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>35</v>
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -753,10 +810,10 @@
         <v>11</v>
       </c>
       <c r="S4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -764,10 +821,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -781,6 +838,9 @@
       <c r="H5" t="s">
         <v>43</v>
       </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
       <c r="L5" t="s">
         <v>23</v>
       </c>
@@ -803,7 +863,7 @@
         <v>44</v>
       </c>
       <c r="T5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -811,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -828,6 +888,9 @@
       <c r="H6" t="s">
         <v>43</v>
       </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
       <c r="L6" t="s">
         <v>23</v>
       </c>
@@ -850,7 +913,7 @@
         <v>44</v>
       </c>
       <c r="T6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -858,22 +921,25 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="H7" t="s">
-        <v>43</v>
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>74</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -882,50 +948,122 @@
         <v>6168</v>
       </c>
       <c r="O7" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="P7" t="s">
         <v>24</v>
       </c>
       <c r="Q7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="R7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="S7" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="T7" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8">
+        <v>6168</v>
+      </c>
+      <c r="O8" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>19</v>
+      </c>
+      <c r="R8" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" t="s">
+        <v>48</v>
+      </c>
+      <c r="T8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L9" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9">
+        <v>6168</v>
+      </c>
+      <c r="O9" t="s">
+        <v>21</v>
+      </c>
+      <c r="P9" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>19</v>
+      </c>
+      <c r="R9" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" t="s">
+        <v>48</v>
+      </c>
+      <c r="T9" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -933,7 +1071,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
@@ -942,13 +1080,16 @@
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
-        <v>48</v>
+        <v>37</v>
+      </c>
+      <c r="I10" t="s">
+        <v>77</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
@@ -957,19 +1098,19 @@
         <v>6168</v>
       </c>
       <c r="O10" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="P10" t="s">
         <v>24</v>
       </c>
       <c r="Q10" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="R10" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="S10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="T10" t="s">
         <v>49</v>
@@ -977,10 +1118,10 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -990,58 +1131,25 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" t="s">
-        <v>48</v>
-      </c>
-      <c r="L12" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12">
-        <v>6168</v>
-      </c>
-      <c r="O12" t="s">
-        <v>20</v>
-      </c>
-      <c r="P12" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>19</v>
-      </c>
-      <c r="R12" t="s">
-        <v>17</v>
-      </c>
-      <c r="S12" t="s">
-        <v>48</v>
-      </c>
-      <c r="T12" t="s">
-        <v>49</v>
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1051,58 +1159,25 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M14">
-        <v>6168</v>
-      </c>
-      <c r="O14" t="s">
-        <v>21</v>
-      </c>
-      <c r="P14" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>19</v>
-      </c>
-      <c r="R14" t="s">
-        <v>17</v>
-      </c>
-      <c r="S14" t="s">
-        <v>48</v>
-      </c>
-      <c r="T14" t="s">
-        <v>40</v>
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1112,50 +1187,17 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>9</v>
-      </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" t="s">
-        <v>37</v>
-      </c>
-      <c r="L16" t="s">
-        <v>23</v>
-      </c>
-      <c r="M16">
-        <v>6168</v>
-      </c>
-      <c r="O16" t="s">
-        <v>15</v>
-      </c>
-      <c r="P16" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>16</v>
-      </c>
-      <c r="R16" t="s">
-        <v>14</v>
-      </c>
-      <c r="S16" t="s">
-        <v>37</v>
-      </c>
-      <c r="T16" t="s">
-        <v>49</v>
+        <v>7</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updating fixtures for scan tests - basic
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_scanned.xlsx
+++ b/tests/fixtures/basic_scanned.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B040A1F9-69D2-4241-9826-59686092553B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7877A4E1-DABB-C24C-BB4E-BD3FE6F1560E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="1520" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="30940" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
   <si>
     <t>File</t>
   </si>
@@ -241,19 +241,22 @@
     <t>DICOM:SeriesNumber</t>
   </si>
   <si>
-    <t>002304_CT1</t>
-  </si>
-  <si>
-    <t>397829_CT1</t>
-  </si>
-  <si>
-    <t>397829_CT2</t>
-  </si>
-  <si>
-    <t>397829_CT3</t>
-  </si>
-  <si>
-    <t>038945_CT1</t>
+    <t>002304_CT1_3</t>
+  </si>
+  <si>
+    <t>002304_CT1_6168</t>
+  </si>
+  <si>
+    <t>397829_CT1_6168</t>
+  </si>
+  <si>
+    <t>397829_CT2_6168</t>
+  </si>
+  <si>
+    <t>397829_CT3_6168</t>
+  </si>
+  <si>
+    <t>038945_CT1_6168</t>
   </si>
 </sst>
 </file>
@@ -596,7 +599,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I10"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -695,7 +698,7 @@
         <v>23</v>
       </c>
       <c r="M2">
-        <v>6168</v>
+        <v>3</v>
       </c>
       <c r="O2" t="s">
         <v>12</v>
@@ -745,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="M3">
-        <v>6168</v>
+        <v>3</v>
       </c>
       <c r="O3" t="s">
         <v>12</v>
@@ -789,7 +792,7 @@
         <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -839,7 +842,7 @@
         <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
@@ -889,7 +892,7 @@
         <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L6" t="s">
         <v>23</v>
@@ -939,7 +942,7 @@
         <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -989,7 +992,7 @@
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
@@ -1039,7 +1042,7 @@
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -1089,7 +1092,7 @@
         <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
updated scan tests to work with strict / not strict scan id collation
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_scanned.xlsx
+++ b/tests/fixtures/basic_scanned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7877A4E1-DABB-C24C-BB4E-BD3FE6F1560E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48EA4F9-C579-C042-ABAA-5CC69A47B8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="500" windowWidth="30940" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6280" yWindow="1520" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
   <si>
     <t>File</t>
   </si>
@@ -241,22 +241,19 @@
     <t>DICOM:SeriesNumber</t>
   </si>
   <si>
-    <t>002304_CT1_3</t>
-  </si>
-  <si>
-    <t>002304_CT1_6168</t>
-  </si>
-  <si>
-    <t>397829_CT1_6168</t>
-  </si>
-  <si>
-    <t>397829_CT2_6168</t>
-  </si>
-  <si>
-    <t>397829_CT3_6168</t>
-  </si>
-  <si>
-    <t>038945_CT1_6168</t>
+    <t>002304_CT1</t>
+  </si>
+  <si>
+    <t>397829_CT1</t>
+  </si>
+  <si>
+    <t>397829_CT2</t>
+  </si>
+  <si>
+    <t>397829_CT3</t>
+  </si>
+  <si>
+    <t>038945_CT1</t>
   </si>
 </sst>
 </file>
@@ -599,7 +596,7 @@
   <dimension ref="A1:T17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -792,7 +789,7 @@
         <v>43</v>
       </c>
       <c r="I4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L4" t="s">
         <v>23</v>
@@ -842,7 +839,7 @@
         <v>43</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L5" t="s">
         <v>23</v>
@@ -892,7 +889,7 @@
         <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L6" t="s">
         <v>23</v>
@@ -942,7 +939,7 @@
         <v>48</v>
       </c>
       <c r="I7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -992,7 +989,7 @@
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
@@ -1042,7 +1039,7 @@
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -1092,7 +1089,7 @@
         <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
The matcher was interpreting the character after the {var} in a pattern like "{filename}.dcm" as a delimiter, and excluding it from the match for the variable, so "{filename}.dcm" would not match a file like "0000.00001.dcm"
Have removed the magic behaviour so it just turns into a regexp which
matches (.*)\.dcm$
</commit_message>
<xml_diff>
--- a/tests/fixtures/basic_scanned.xlsx
+++ b/tests/fixtures/basic_scanned.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48EA4F9-C579-C042-ABAA-5CC69A47B8B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13D5C9F-9031-1D4E-BFDE-D887B96D0352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="1520" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6720" yWindow="6820" windowWidth="30680" windowHeight="18300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Files" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="81">
   <si>
     <t>File</t>
   </si>
@@ -254,6 +254,15 @@
   </si>
   <si>
     <t>038945_CT1</t>
+  </si>
+  <si>
+    <t>tests/fixtures/basic/DOE^JOHN-002304/20200312HeadCT/Head CT/image-00002.extra.periods.dcm</t>
+  </si>
+  <si>
+    <t>image-00002.extra.periods.dcm</t>
+  </si>
+  <si>
+    <t>image-00002.extra.periods</t>
   </si>
 </sst>
 </file>
@@ -593,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCC7506-3A8B-3C43-9E0E-9F3B5EB91639}">
-  <dimension ref="A1:T17"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -771,10 +780,10 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>79</v>
       </c>
       <c r="D4" t="s">
         <v>10</v>
@@ -786,7 +795,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
         <v>73</v>
@@ -795,7 +804,7 @@
         <v>23</v>
       </c>
       <c r="M4">
-        <v>6168</v>
+        <v>3</v>
       </c>
       <c r="O4" t="s">
         <v>12</v>
@@ -810,10 +819,10 @@
         <v>11</v>
       </c>
       <c r="S4" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="T4" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
@@ -821,10 +830,10 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -863,7 +872,7 @@
         <v>44</v>
       </c>
       <c r="T5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
@@ -871,10 +880,10 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>10</v>
@@ -913,7 +922,7 @@
         <v>44</v>
       </c>
       <c r="T6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
@@ -921,25 +930,25 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D7" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="I7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L7" t="s">
         <v>23</v>
@@ -948,22 +957,22 @@
         <v>6168</v>
       </c>
       <c r="O7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="P7" t="s">
         <v>24</v>
       </c>
       <c r="Q7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="R7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="S7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="T7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
@@ -971,7 +980,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>47</v>
@@ -983,13 +992,13 @@
         <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H8" t="s">
         <v>48</v>
       </c>
       <c r="I8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
@@ -998,7 +1007,7 @@
         <v>6168</v>
       </c>
       <c r="O8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="P8" t="s">
         <v>24</v>
@@ -1021,10 +1030,10 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -1033,13 +1042,13 @@
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H9" t="s">
         <v>48</v>
       </c>
       <c r="I9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -1048,7 +1057,7 @@
         <v>6168</v>
       </c>
       <c r="O9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P9" t="s">
         <v>24</v>
@@ -1063,7 +1072,7 @@
         <v>48</v>
       </c>
       <c r="T9" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
@@ -1071,25 +1080,25 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="I10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
@@ -1098,44 +1107,80 @@
         <v>6168</v>
       </c>
       <c r="O10" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="P10" t="s">
         <v>24</v>
       </c>
       <c r="Q10" t="s">
+        <v>19</v>
+      </c>
+      <c r="R10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S10" t="s">
+        <v>48</v>
+      </c>
+      <c r="T10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" t="s">
+        <v>23</v>
+      </c>
+      <c r="M11">
+        <v>6168</v>
+      </c>
+      <c r="O11" t="s">
+        <v>15</v>
+      </c>
+      <c r="P11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q11" t="s">
         <v>16</v>
       </c>
-      <c r="R10" t="s">
+      <c r="R11" t="s">
         <v>14</v>
       </c>
-      <c r="S10" t="s">
+      <c r="S11" t="s">
         <v>37</v>
       </c>
-      <c r="T10" t="s">
+      <c r="T11" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -1146,10 +1191,10 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -1160,10 +1205,10 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -1174,10 +1219,10 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -1188,10 +1233,10 @@
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -1202,15 +1247,29 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>